<commit_message>
fix sedtrap data import error
</commit_message>
<xml_diff>
--- a/data/sediment_traps/Baseline sediment tables and charts- reef 3 31114.xlsx
+++ b/data/sediment_traps/Baseline sediment tables and charts- reef 3 31114.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11109"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dial Cordy\Documents\Data\Baseline\Reef 3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jrcunning/Projects/pom-dredge/data/sediment_traps/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{EF2BF500-6BC4-B441-8D2B-86CED5C0FB28}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11985" activeTab="2"/>
+    <workbookView xWindow="180" yWindow="1460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="baseline" sheetId="1" r:id="rId1"/>
@@ -20,7 +21,14 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">baseline!$B$2:$S$50</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -51,165 +59,87 @@
     <t>HBNC T3</t>
   </si>
   <si>
-    <t>HBN1T1</t>
-  </si>
-  <si>
     <t>E</t>
   </si>
   <si>
-    <t>HBN1T2</t>
-  </si>
-  <si>
     <t>F</t>
   </si>
   <si>
-    <t>HBN1T3</t>
-  </si>
-  <si>
     <t>G</t>
   </si>
   <si>
-    <t>HBS1T1</t>
-  </si>
-  <si>
     <t>H</t>
   </si>
   <si>
-    <t>HBS1T2</t>
-  </si>
-  <si>
     <t>I</t>
   </si>
   <si>
-    <t>HBS1T3</t>
-  </si>
-  <si>
     <t>J</t>
   </si>
   <si>
-    <t>HBS2T1</t>
-  </si>
-  <si>
     <t>Tree was laying on side when collection made.</t>
   </si>
   <si>
     <t>K</t>
   </si>
   <si>
-    <t>HBS2T2</t>
-  </si>
-  <si>
     <t>L</t>
   </si>
   <si>
-    <t>HBS2T3</t>
-  </si>
-  <si>
     <t>M</t>
   </si>
   <si>
-    <t>HBN2T1</t>
-  </si>
-  <si>
     <t>N</t>
   </si>
   <si>
-    <t>HBN2T2</t>
-  </si>
-  <si>
     <t>O</t>
   </si>
   <si>
-    <t>HBN2T3</t>
-  </si>
-  <si>
     <t>P</t>
   </si>
   <si>
-    <t>HBN3T1</t>
-  </si>
-  <si>
     <t>Q</t>
   </si>
   <si>
-    <t>HBN3T2</t>
-  </si>
-  <si>
     <t>R</t>
   </si>
   <si>
     <t>S</t>
   </si>
   <si>
-    <t>HBS3T1</t>
-  </si>
-  <si>
     <t>T</t>
   </si>
   <si>
-    <t>HBS3T2</t>
-  </si>
-  <si>
     <t>U</t>
   </si>
   <si>
-    <t>HBS3T3</t>
-  </si>
-  <si>
     <t>V</t>
   </si>
   <si>
-    <t>HBS4T1</t>
-  </si>
-  <si>
     <t>W</t>
   </si>
   <si>
-    <t>HBS4T2</t>
-  </si>
-  <si>
     <t>X</t>
   </si>
   <si>
-    <t>HBS4T3</t>
-  </si>
-  <si>
     <t>Y</t>
   </si>
   <si>
-    <t>HBSC1T1</t>
-  </si>
-  <si>
     <t>Z</t>
   </si>
   <si>
-    <t>HBSC1T2</t>
-  </si>
-  <si>
     <t>AA</t>
   </si>
   <si>
-    <t>HBSC1T3</t>
-  </si>
-  <si>
     <t>BB</t>
   </si>
   <si>
-    <t>R2SC1T1</t>
-  </si>
-  <si>
     <t>CC</t>
   </si>
   <si>
-    <t>R2SC1T2</t>
-  </si>
-  <si>
     <t>DD</t>
   </si>
   <si>
-    <t>R2SC1T3</t>
-  </si>
-  <si>
     <t>EE</t>
   </si>
   <si>
@@ -237,24 +167,6 @@
     <t>R2NC1-LR T3</t>
   </si>
   <si>
-    <t>R2S1T1</t>
-  </si>
-  <si>
-    <t>R2S1T2</t>
-  </si>
-  <si>
-    <t>R2S1T3</t>
-  </si>
-  <si>
-    <t>R2N1T1</t>
-  </si>
-  <si>
-    <t>R2N1T2</t>
-  </si>
-  <si>
-    <t>R2N1T3</t>
-  </si>
-  <si>
     <t>Site Name-Transect</t>
   </si>
   <si>
@@ -289,9 +201,6 @@
   </si>
   <si>
     <t>Total Wet Mass                  (grams)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HBN3T3                        </t>
   </si>
   <si>
     <t>Dry Mass Retained on No. 230 Sieve and Tare (grams)</t>
@@ -611,11 +520,110 @@
       <t xml:space="preserve"> 230) </t>
     </r>
   </si>
+  <si>
+    <t>HBN1 T1</t>
+  </si>
+  <si>
+    <t>HBN1 T2</t>
+  </si>
+  <si>
+    <t>HBN1 T3</t>
+  </si>
+  <si>
+    <t>HBS1 T1</t>
+  </si>
+  <si>
+    <t>HBS1 T2</t>
+  </si>
+  <si>
+    <t>HBS1 T3</t>
+  </si>
+  <si>
+    <t>HBS2 T1</t>
+  </si>
+  <si>
+    <t>HBS2 T2</t>
+  </si>
+  <si>
+    <t>HBS2 T3</t>
+  </si>
+  <si>
+    <t>HBN2 T1</t>
+  </si>
+  <si>
+    <t>HBN2 T2</t>
+  </si>
+  <si>
+    <t>HBN2 T3</t>
+  </si>
+  <si>
+    <t>HBN3 T1</t>
+  </si>
+  <si>
+    <t>HBN3 T2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HBN3 T3                        </t>
+  </si>
+  <si>
+    <t>HBS3 T1</t>
+  </si>
+  <si>
+    <t>HBS3 T2</t>
+  </si>
+  <si>
+    <t>HBS3 T3</t>
+  </si>
+  <si>
+    <t>HBS4 T1</t>
+  </si>
+  <si>
+    <t>HBS4 T2</t>
+  </si>
+  <si>
+    <t>HBS4 T3</t>
+  </si>
+  <si>
+    <t>HBSC1 T1</t>
+  </si>
+  <si>
+    <t>HBSC1 T2</t>
+  </si>
+  <si>
+    <t>HBSC1 T3</t>
+  </si>
+  <si>
+    <t>R2SC1 T1</t>
+  </si>
+  <si>
+    <t>R2SC1 T2</t>
+  </si>
+  <si>
+    <t>R2SC1 T3</t>
+  </si>
+  <si>
+    <t>R2S1 T1</t>
+  </si>
+  <si>
+    <t>R2S1 T2</t>
+  </si>
+  <si>
+    <t>R2S1 T3</t>
+  </si>
+  <si>
+    <t>R2N1 T1</t>
+  </si>
+  <si>
+    <t>R2N1 T2</t>
+  </si>
+  <si>
+    <t>R2N1 T3</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="mm/dd/yy;@"/>
@@ -1741,6 +1749,51 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="4"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -1768,49 +1821,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1818,9 +1829,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
@@ -1858,7 +1866,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2079,6 +2087,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-9D5E-C742-BC33-AFC1BD59DAE7}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -2191,7 +2204,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2304,7 +2316,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2517,6 +2529,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F601-6A47-8B94-46713DE6953A}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -2629,7 +2646,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3842,7 +3858,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -3872,7 +3894,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -3966,6 +3994,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -4001,6 +4046,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -4176,176 +4238,177 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A2:T53"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection sqref="A1:S50"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.5703125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="7.5" style="2" customWidth="1"/>
+    <col min="2" max="2" width="13.1640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="11.1640625" style="2" customWidth="1"/>
     <col min="4" max="4" width="14" style="2" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="18.5703125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="11.140625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="12.85546875" style="2" customWidth="1"/>
-    <col min="9" max="9" width="11.140625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="10.7109375" style="2" customWidth="1"/>
-    <col min="11" max="11" width="9.5703125" style="2" customWidth="1"/>
-    <col min="12" max="12" width="12.7109375" style="2" customWidth="1"/>
-    <col min="13" max="13" width="8.7109375" style="2" customWidth="1"/>
-    <col min="14" max="14" width="12.5703125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="15.5" style="2" customWidth="1"/>
+    <col min="6" max="6" width="18.5" style="2" customWidth="1"/>
+    <col min="7" max="7" width="11.1640625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="12.83203125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="11.1640625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="10.6640625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="9.5" style="2" customWidth="1"/>
+    <col min="12" max="12" width="12.6640625" style="2" customWidth="1"/>
+    <col min="13" max="13" width="8.6640625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="12.5" style="2" customWidth="1"/>
     <col min="15" max="15" width="12" style="2" customWidth="1"/>
-    <col min="16" max="16" width="14.7109375" style="2" customWidth="1"/>
-    <col min="17" max="17" width="9.140625" style="2" customWidth="1"/>
-    <col min="18" max="18" width="13.85546875" style="2" customWidth="1"/>
-    <col min="19" max="19" width="14.7109375" style="2" customWidth="1"/>
-    <col min="21" max="16384" width="9.140625" style="2"/>
+    <col min="16" max="16" width="14.6640625" style="2" customWidth="1"/>
+    <col min="17" max="17" width="9.1640625" style="2" customWidth="1"/>
+    <col min="18" max="18" width="13.83203125" style="2" customWidth="1"/>
+    <col min="19" max="19" width="14.6640625" style="2" customWidth="1"/>
+    <col min="20" max="20" width="8.83203125" customWidth="1"/>
+    <col min="21" max="16384" width="9.1640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="139" t="s">
-        <v>95</v>
-      </c>
-      <c r="C2" s="140"/>
-      <c r="D2" s="140"/>
-      <c r="E2" s="140"/>
-      <c r="F2" s="140"/>
-      <c r="G2" s="140"/>
-      <c r="H2" s="140"/>
-      <c r="I2" s="140"/>
-      <c r="J2" s="140"/>
-      <c r="K2" s="140"/>
-      <c r="L2" s="140"/>
-      <c r="M2" s="140"/>
-      <c r="N2" s="140"/>
-      <c r="O2" s="140"/>
-      <c r="P2" s="140"/>
-      <c r="Q2" s="140"/>
-      <c r="R2" s="140"/>
-      <c r="S2" s="140"/>
-    </row>
-    <row r="3" spans="1:20" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="130" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" s="131"/>
+      <c r="D2" s="131"/>
+      <c r="E2" s="131"/>
+      <c r="F2" s="131"/>
+      <c r="G2" s="131"/>
+      <c r="H2" s="131"/>
+      <c r="I2" s="131"/>
+      <c r="J2" s="131"/>
+      <c r="K2" s="131"/>
+      <c r="L2" s="131"/>
+      <c r="M2" s="131"/>
+      <c r="N2" s="131"/>
+      <c r="O2" s="131"/>
+      <c r="P2" s="131"/>
+      <c r="Q2" s="131"/>
+      <c r="R2" s="131"/>
+      <c r="S2" s="131"/>
+    </row>
+    <row r="3" spans="1:20" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="T3" s="2"/>
     </row>
-    <row r="4" spans="1:20" ht="29.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20" ht="29.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
-      <c r="B4" s="134" t="s">
-        <v>84</v>
-      </c>
-      <c r="C4" s="135"/>
-      <c r="D4" s="135"/>
-      <c r="E4" s="135"/>
-      <c r="F4" s="135"/>
-      <c r="G4" s="136" t="s">
-        <v>85</v>
-      </c>
-      <c r="H4" s="137"/>
-      <c r="I4" s="137"/>
-      <c r="J4" s="137"/>
-      <c r="K4" s="137"/>
-      <c r="L4" s="137"/>
-      <c r="M4" s="137"/>
-      <c r="N4" s="137"/>
-      <c r="O4" s="137"/>
-      <c r="P4" s="137"/>
-      <c r="Q4" s="137"/>
-      <c r="R4" s="137"/>
-      <c r="S4" s="138"/>
+      <c r="B4" s="149" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" s="150"/>
+      <c r="D4" s="150"/>
+      <c r="E4" s="150"/>
+      <c r="F4" s="150"/>
+      <c r="G4" s="151" t="s">
+        <v>53</v>
+      </c>
+      <c r="H4" s="152"/>
+      <c r="I4" s="152"/>
+      <c r="J4" s="152"/>
+      <c r="K4" s="152"/>
+      <c r="L4" s="152"/>
+      <c r="M4" s="152"/>
+      <c r="N4" s="152"/>
+      <c r="O4" s="152"/>
+      <c r="P4" s="152"/>
+      <c r="Q4" s="152"/>
+      <c r="R4" s="152"/>
+      <c r="S4" s="153"/>
       <c r="T4" s="2"/>
     </row>
-    <row r="5" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3"/>
-      <c r="B5" s="141" t="s">
+      <c r="B5" s="132" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="145" t="s">
+      <c r="C5" s="136" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="145" t="s">
-        <v>79</v>
-      </c>
-      <c r="E5" s="145" t="s">
-        <v>76</v>
-      </c>
-      <c r="F5" s="143" t="s">
-        <v>77</v>
-      </c>
-      <c r="G5" s="132" t="s">
-        <v>96</v>
-      </c>
-      <c r="H5" s="147" t="s">
-        <v>87</v>
-      </c>
-      <c r="I5" s="148" t="s">
-        <v>86</v>
-      </c>
-      <c r="J5" s="148" t="s">
-        <v>81</v>
-      </c>
-      <c r="K5" s="148" t="s">
-        <v>83</v>
-      </c>
-      <c r="L5" s="149" t="s">
-        <v>93</v>
-      </c>
-      <c r="M5" s="150"/>
-      <c r="N5" s="151"/>
-      <c r="O5" s="149" t="s">
-        <v>94</v>
-      </c>
-      <c r="P5" s="152"/>
-      <c r="Q5" s="152"/>
-      <c r="R5" s="152"/>
-      <c r="S5" s="153"/>
+      <c r="D5" s="136" t="s">
+        <v>47</v>
+      </c>
+      <c r="E5" s="136" t="s">
+        <v>44</v>
+      </c>
+      <c r="F5" s="134" t="s">
+        <v>45</v>
+      </c>
+      <c r="G5" s="147" t="s">
+        <v>63</v>
+      </c>
+      <c r="H5" s="138" t="s">
+        <v>55</v>
+      </c>
+      <c r="I5" s="139" t="s">
+        <v>54</v>
+      </c>
+      <c r="J5" s="139" t="s">
+        <v>49</v>
+      </c>
+      <c r="K5" s="139" t="s">
+        <v>51</v>
+      </c>
+      <c r="L5" s="140" t="s">
+        <v>60</v>
+      </c>
+      <c r="M5" s="141"/>
+      <c r="N5" s="142"/>
+      <c r="O5" s="140" t="s">
+        <v>61</v>
+      </c>
+      <c r="P5" s="143"/>
+      <c r="Q5" s="143"/>
+      <c r="R5" s="143"/>
+      <c r="S5" s="144"/>
       <c r="T5" s="2"/>
     </row>
-    <row r="6" spans="1:20" ht="68.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:20" ht="68.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
-      <c r="B6" s="142"/>
-      <c r="C6" s="146"/>
-      <c r="D6" s="146"/>
-      <c r="E6" s="146"/>
-      <c r="F6" s="144"/>
-      <c r="G6" s="133"/>
-      <c r="H6" s="144"/>
-      <c r="I6" s="146"/>
-      <c r="J6" s="146"/>
-      <c r="K6" s="146"/>
+      <c r="B6" s="133"/>
+      <c r="C6" s="137"/>
+      <c r="D6" s="137"/>
+      <c r="E6" s="137"/>
+      <c r="F6" s="135"/>
+      <c r="G6" s="148"/>
+      <c r="H6" s="135"/>
+      <c r="I6" s="137"/>
+      <c r="J6" s="137"/>
+      <c r="K6" s="137"/>
       <c r="L6" s="25" t="s">
-        <v>89</v>
+        <v>56</v>
       </c>
       <c r="M6" s="26" t="s">
-        <v>78</v>
+        <v>46</v>
       </c>
       <c r="N6" s="27" t="s">
-        <v>90</v>
+        <v>57</v>
       </c>
       <c r="O6" s="27" t="s">
-        <v>101</v>
+        <v>68</v>
       </c>
       <c r="P6" s="26" t="s">
-        <v>91</v>
+        <v>58</v>
       </c>
       <c r="Q6" s="26" t="s">
-        <v>78</v>
+        <v>46</v>
       </c>
       <c r="R6" s="27" t="s">
-        <v>100</v>
+        <v>67</v>
       </c>
       <c r="S6" s="28" t="s">
-        <v>80</v>
+        <v>48</v>
       </c>
       <c r="T6" s="2"/>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7" s="3"/>
       <c r="B7" s="4" t="s">
         <v>2</v>
@@ -4407,7 +4470,7 @@
       </c>
       <c r="T7" s="2"/>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A8" s="3"/>
       <c r="B8" s="4" t="s">
         <v>4</v>
@@ -4469,7 +4532,7 @@
       </c>
       <c r="T8" s="2"/>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A9" s="3"/>
       <c r="B9" s="12" t="s">
         <v>6</v>
@@ -4484,7 +4547,7 @@
         <v>7</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>99</v>
+        <v>66</v>
       </c>
       <c r="G9" s="36">
         <v>41638</v>
@@ -4533,10 +4596,10 @@
       </c>
       <c r="T9" s="2"/>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A10" s="3"/>
       <c r="B10" s="4" t="s">
-        <v>99</v>
+        <v>66</v>
       </c>
       <c r="C10" s="5">
         <v>3</v>
@@ -4545,7 +4608,7 @@
         <v>41596</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>8</v>
+        <v>148</v>
       </c>
       <c r="F10" s="17"/>
       <c r="G10" s="35">
@@ -4595,10 +4658,10 @@
       </c>
       <c r="T10" s="2"/>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A11" s="3"/>
       <c r="B11" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C11" s="5">
         <v>3</v>
@@ -4607,7 +4670,7 @@
         <v>41596</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>10</v>
+        <v>149</v>
       </c>
       <c r="F11" s="17"/>
       <c r="G11" s="35">
@@ -4657,10 +4720,10 @@
       </c>
       <c r="T11" s="2"/>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A12" s="3"/>
       <c r="B12" s="12" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C12" s="13">
         <v>3</v>
@@ -4669,7 +4732,7 @@
         <v>41596</v>
       </c>
       <c r="E12" s="15" t="s">
-        <v>12</v>
+        <v>150</v>
       </c>
       <c r="F12" s="18"/>
       <c r="G12" s="36">
@@ -4719,10 +4782,10 @@
       </c>
       <c r="T12" s="2"/>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A13" s="3"/>
       <c r="B13" s="4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C13" s="5">
         <v>3</v>
@@ -4731,7 +4794,7 @@
         <v>41596</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>14</v>
+        <v>151</v>
       </c>
       <c r="F13" s="17"/>
       <c r="G13" s="35">
@@ -4781,10 +4844,10 @@
       </c>
       <c r="T13" s="2"/>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A14" s="3"/>
       <c r="B14" s="4" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C14" s="5">
         <v>3</v>
@@ -4793,7 +4856,7 @@
         <v>41596</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>16</v>
+        <v>152</v>
       </c>
       <c r="F14" s="17"/>
       <c r="G14" s="35">
@@ -4843,10 +4906,10 @@
       </c>
       <c r="T14" s="2"/>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A15" s="3"/>
       <c r="B15" s="12" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C15" s="13">
         <v>3</v>
@@ -4855,7 +4918,7 @@
         <v>41596</v>
       </c>
       <c r="E15" s="15" t="s">
-        <v>18</v>
+        <v>153</v>
       </c>
       <c r="F15" s="18"/>
       <c r="G15" s="36">
@@ -4905,10 +4968,10 @@
       </c>
       <c r="T15" s="2"/>
     </row>
-    <row r="16" spans="1:20" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3"/>
       <c r="B16" s="4" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C16" s="5">
         <v>3</v>
@@ -4917,10 +4980,10 @@
         <v>41596</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>20</v>
+        <v>154</v>
       </c>
       <c r="F16" s="19" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="G16" s="35">
         <v>41638</v>
@@ -4969,10 +5032,10 @@
       </c>
       <c r="T16" s="2"/>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A17" s="3"/>
       <c r="B17" s="4" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C17" s="5">
         <v>3</v>
@@ -4981,7 +5044,7 @@
         <v>41596</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>23</v>
+        <v>155</v>
       </c>
       <c r="F17" s="20"/>
       <c r="G17" s="35">
@@ -5031,10 +5094,10 @@
       </c>
       <c r="T17" s="2"/>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A18" s="3"/>
       <c r="B18" s="12" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="C18" s="13">
         <v>3</v>
@@ -5043,7 +5106,7 @@
         <v>41596</v>
       </c>
       <c r="E18" s="15" t="s">
-        <v>25</v>
+        <v>156</v>
       </c>
       <c r="F18" s="21"/>
       <c r="G18" s="36">
@@ -5093,10 +5156,10 @@
       </c>
       <c r="T18" s="2"/>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A19" s="3"/>
       <c r="B19" s="4" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="C19" s="5">
         <v>3</v>
@@ -5105,7 +5168,7 @@
         <v>41596</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>27</v>
+        <v>157</v>
       </c>
       <c r="F19" s="20"/>
       <c r="G19" s="35">
@@ -5155,10 +5218,10 @@
       </c>
       <c r="T19" s="2"/>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A20" s="3"/>
       <c r="B20" s="4" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="C20" s="5">
         <v>3</v>
@@ -5167,7 +5230,7 @@
         <v>41596</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>29</v>
+        <v>158</v>
       </c>
       <c r="F20" s="20"/>
       <c r="G20" s="35">
@@ -5217,10 +5280,10 @@
       </c>
       <c r="T20" s="2"/>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A21" s="3"/>
       <c r="B21" s="12" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="C21" s="13">
         <v>3</v>
@@ -5229,7 +5292,7 @@
         <v>41596</v>
       </c>
       <c r="E21" s="15" t="s">
-        <v>31</v>
+        <v>159</v>
       </c>
       <c r="F21" s="21"/>
       <c r="G21" s="36">
@@ -5279,10 +5342,10 @@
       </c>
       <c r="T21" s="2"/>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A22" s="3"/>
       <c r="B22" s="4" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="C22" s="5">
         <v>3</v>
@@ -5291,7 +5354,7 @@
         <v>41596</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>33</v>
+        <v>160</v>
       </c>
       <c r="F22" s="20"/>
       <c r="G22" s="35">
@@ -5341,10 +5404,10 @@
       </c>
       <c r="T22" s="2"/>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A23" s="3"/>
       <c r="B23" s="4" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="C23" s="5">
         <v>3</v>
@@ -5353,7 +5416,7 @@
         <v>41596</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>35</v>
+        <v>161</v>
       </c>
       <c r="F23" s="20"/>
       <c r="G23" s="35">
@@ -5403,68 +5466,68 @@
       </c>
       <c r="T23" s="2"/>
     </row>
-    <row r="24" spans="1:20" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:20" ht="24" x14ac:dyDescent="0.2">
       <c r="A24" s="3"/>
       <c r="B24" s="12" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="C24" s="16" t="s">
-        <v>82</v>
+        <v>50</v>
       </c>
       <c r="D24" s="16" t="s">
-        <v>82</v>
+        <v>50</v>
       </c>
       <c r="E24" s="15" t="s">
-        <v>88</v>
+        <v>162</v>
       </c>
       <c r="F24" s="22" t="s">
-        <v>92</v>
+        <v>59</v>
       </c>
       <c r="G24" s="43" t="s">
-        <v>82</v>
+        <v>50</v>
       </c>
       <c r="H24" s="39" t="s">
-        <v>82</v>
+        <v>50</v>
       </c>
       <c r="I24" s="40" t="s">
-        <v>82</v>
+        <v>50</v>
       </c>
       <c r="J24" s="16" t="s">
-        <v>82</v>
+        <v>50</v>
       </c>
       <c r="K24" s="41" t="s">
-        <v>82</v>
+        <v>50</v>
       </c>
       <c r="L24" s="16" t="s">
-        <v>82</v>
+        <v>50</v>
       </c>
       <c r="M24" s="16" t="s">
-        <v>82</v>
+        <v>50</v>
       </c>
       <c r="N24" s="16" t="s">
-        <v>82</v>
+        <v>50</v>
       </c>
       <c r="O24" s="16" t="s">
-        <v>82</v>
+        <v>50</v>
       </c>
       <c r="P24" s="16" t="s">
-        <v>82</v>
+        <v>50</v>
       </c>
       <c r="Q24" s="16" t="s">
-        <v>82</v>
+        <v>50</v>
       </c>
       <c r="R24" s="16" t="s">
-        <v>82</v>
+        <v>50</v>
       </c>
       <c r="S24" s="42" t="s">
-        <v>82</v>
+        <v>50</v>
       </c>
       <c r="T24" s="2"/>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A25" s="3"/>
       <c r="B25" s="4" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="C25" s="5">
         <v>3</v>
@@ -5473,7 +5536,7 @@
         <v>41596</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>38</v>
+        <v>163</v>
       </c>
       <c r="F25" s="17"/>
       <c r="G25" s="35">
@@ -5523,10 +5586,10 @@
       </c>
       <c r="T25" s="2"/>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A26" s="3"/>
       <c r="B26" s="4" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="C26" s="5">
         <v>3</v>
@@ -5535,7 +5598,7 @@
         <v>41596</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>40</v>
+        <v>164</v>
       </c>
       <c r="F26" s="17"/>
       <c r="G26" s="35">
@@ -5585,10 +5648,10 @@
       </c>
       <c r="T26" s="2"/>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A27" s="3"/>
       <c r="B27" s="12" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="C27" s="13">
         <v>3</v>
@@ -5597,7 +5660,7 @@
         <v>41596</v>
       </c>
       <c r="E27" s="15" t="s">
-        <v>42</v>
+        <v>165</v>
       </c>
       <c r="F27" s="18"/>
       <c r="G27" s="36">
@@ -5647,10 +5710,10 @@
       </c>
       <c r="T27" s="2"/>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A28" s="3"/>
       <c r="B28" s="4" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="C28" s="5">
         <v>3</v>
@@ -5659,7 +5722,7 @@
         <v>41596</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>44</v>
+        <v>166</v>
       </c>
       <c r="F28" s="17"/>
       <c r="G28" s="35">
@@ -5709,10 +5772,10 @@
       </c>
       <c r="T28" s="2"/>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A29" s="3"/>
       <c r="B29" s="4" t="s">
-        <v>45</v>
+        <v>27</v>
       </c>
       <c r="C29" s="5">
         <v>3</v>
@@ -5721,7 +5784,7 @@
         <v>41596</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>46</v>
+        <v>167</v>
       </c>
       <c r="F29" s="17"/>
       <c r="G29" s="35">
@@ -5771,10 +5834,10 @@
       </c>
       <c r="T29" s="2"/>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A30" s="3"/>
       <c r="B30" s="12" t="s">
-        <v>47</v>
+        <v>28</v>
       </c>
       <c r="C30" s="13">
         <v>3</v>
@@ -5783,7 +5846,7 @@
         <v>41596</v>
       </c>
       <c r="E30" s="15" t="s">
-        <v>48</v>
+        <v>168</v>
       </c>
       <c r="F30" s="18"/>
       <c r="G30" s="36">
@@ -5833,10 +5896,10 @@
       </c>
       <c r="T30" s="2"/>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A31" s="3"/>
       <c r="B31" s="4" t="s">
-        <v>49</v>
+        <v>29</v>
       </c>
       <c r="C31" s="5">
         <v>3</v>
@@ -5845,7 +5908,7 @@
         <v>41596</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>50</v>
+        <v>169</v>
       </c>
       <c r="F31" s="17"/>
       <c r="G31" s="35">
@@ -5895,10 +5958,10 @@
       </c>
       <c r="T31" s="2"/>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A32" s="3"/>
       <c r="B32" s="4" t="s">
-        <v>51</v>
+        <v>30</v>
       </c>
       <c r="C32" s="5">
         <v>3</v>
@@ -5907,7 +5970,7 @@
         <v>41596</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>52</v>
+        <v>170</v>
       </c>
       <c r="F32" s="17"/>
       <c r="G32" s="35">
@@ -5957,10 +6020,10 @@
       </c>
       <c r="T32" s="2"/>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A33" s="3"/>
       <c r="B33" s="12" t="s">
-        <v>53</v>
+        <v>31</v>
       </c>
       <c r="C33" s="13">
         <v>3</v>
@@ -5969,7 +6032,7 @@
         <v>41596</v>
       </c>
       <c r="E33" s="15" t="s">
-        <v>54</v>
+        <v>171</v>
       </c>
       <c r="F33" s="18"/>
       <c r="G33" s="36">
@@ -6019,10 +6082,10 @@
       </c>
       <c r="T33" s="2"/>
     </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A34" s="3"/>
       <c r="B34" s="4" t="s">
-        <v>55</v>
+        <v>32</v>
       </c>
       <c r="C34" s="5">
         <v>3</v>
@@ -6031,7 +6094,7 @@
         <v>41596</v>
       </c>
       <c r="E34" s="7" t="s">
-        <v>56</v>
+        <v>172</v>
       </c>
       <c r="F34" s="17"/>
       <c r="G34" s="35">
@@ -6081,10 +6144,10 @@
       </c>
       <c r="T34" s="2"/>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A35" s="3"/>
       <c r="B35" s="4" t="s">
-        <v>57</v>
+        <v>33</v>
       </c>
       <c r="C35" s="5">
         <v>3</v>
@@ -6093,7 +6156,7 @@
         <v>41596</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>58</v>
+        <v>173</v>
       </c>
       <c r="F35" s="17"/>
       <c r="G35" s="35">
@@ -6143,10 +6206,10 @@
       </c>
       <c r="T35" s="2"/>
     </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A36" s="3"/>
       <c r="B36" s="12" t="s">
-        <v>59</v>
+        <v>34</v>
       </c>
       <c r="C36" s="13">
         <v>3</v>
@@ -6155,7 +6218,7 @@
         <v>41596</v>
       </c>
       <c r="E36" s="15" t="s">
-        <v>60</v>
+        <v>174</v>
       </c>
       <c r="F36" s="18"/>
       <c r="G36" s="36">
@@ -6205,10 +6268,10 @@
       </c>
       <c r="T36" s="2"/>
     </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A37" s="3"/>
       <c r="B37" s="4" t="s">
-        <v>61</v>
+        <v>35</v>
       </c>
       <c r="C37" s="5">
         <v>3</v>
@@ -6217,7 +6280,7 @@
         <v>41596</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>70</v>
+        <v>175</v>
       </c>
       <c r="F37" s="17"/>
       <c r="G37" s="35">
@@ -6267,10 +6330,10 @@
       </c>
       <c r="T37" s="2"/>
     </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A38" s="3"/>
       <c r="B38" s="4" t="s">
-        <v>62</v>
+        <v>36</v>
       </c>
       <c r="C38" s="5">
         <v>3</v>
@@ -6279,7 +6342,7 @@
         <v>41596</v>
       </c>
       <c r="E38" s="7" t="s">
-        <v>71</v>
+        <v>176</v>
       </c>
       <c r="F38" s="17"/>
       <c r="G38" s="35">
@@ -6329,10 +6392,10 @@
       </c>
       <c r="T38" s="2"/>
     </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A39" s="3"/>
       <c r="B39" s="12" t="s">
-        <v>63</v>
+        <v>37</v>
       </c>
       <c r="C39" s="13">
         <v>3</v>
@@ -6341,7 +6404,7 @@
         <v>41596</v>
       </c>
       <c r="E39" s="15" t="s">
-        <v>72</v>
+        <v>177</v>
       </c>
       <c r="F39" s="18"/>
       <c r="G39" s="36">
@@ -6391,10 +6454,10 @@
       </c>
       <c r="T39" s="2"/>
     </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A40" s="3"/>
       <c r="B40" s="4" t="s">
-        <v>64</v>
+        <v>38</v>
       </c>
       <c r="C40" s="5">
         <v>3</v>
@@ -6403,7 +6466,7 @@
         <v>41596</v>
       </c>
       <c r="E40" s="7" t="s">
-        <v>73</v>
+        <v>178</v>
       </c>
       <c r="F40" s="17"/>
       <c r="G40" s="35">
@@ -6453,10 +6516,10 @@
       </c>
       <c r="T40" s="2"/>
     </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A41" s="3"/>
       <c r="B41" s="4" t="s">
-        <v>65</v>
+        <v>39</v>
       </c>
       <c r="C41" s="5">
         <v>3</v>
@@ -6465,7 +6528,7 @@
         <v>41596</v>
       </c>
       <c r="E41" s="7" t="s">
-        <v>74</v>
+        <v>179</v>
       </c>
       <c r="F41" s="17"/>
       <c r="G41" s="35">
@@ -6515,10 +6578,10 @@
       </c>
       <c r="T41" s="2"/>
     </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A42" s="3"/>
       <c r="B42" s="12" t="s">
-        <v>66</v>
+        <v>40</v>
       </c>
       <c r="C42" s="13">
         <v>3</v>
@@ -6527,7 +6590,7 @@
         <v>41596</v>
       </c>
       <c r="E42" s="15" t="s">
-        <v>75</v>
+        <v>180</v>
       </c>
       <c r="F42" s="18"/>
       <c r="G42" s="36">
@@ -6577,10 +6640,10 @@
       </c>
       <c r="T42" s="2"/>
     </row>
-    <row r="43" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="3"/>
       <c r="B43" s="4" t="s">
-        <v>67</v>
+        <v>41</v>
       </c>
       <c r="C43" s="5">
         <v>3</v>
@@ -6589,7 +6652,7 @@
         <v>41602</v>
       </c>
       <c r="E43" s="7" t="s">
-        <v>67</v>
+        <v>41</v>
       </c>
       <c r="F43" s="23"/>
       <c r="G43" s="37">
@@ -6639,10 +6702,10 @@
       </c>
       <c r="T43" s="2"/>
     </row>
-    <row r="44" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="3"/>
       <c r="B44" s="4" t="s">
-        <v>68</v>
+        <v>42</v>
       </c>
       <c r="C44" s="5">
         <v>2</v>
@@ -6651,7 +6714,7 @@
         <v>41602</v>
       </c>
       <c r="E44" s="7" t="s">
-        <v>68</v>
+        <v>42</v>
       </c>
       <c r="F44" s="23"/>
       <c r="G44" s="37">
@@ -6701,10 +6764,10 @@
       </c>
       <c r="T44" s="2"/>
     </row>
-    <row r="45" spans="1:20" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:20" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A45" s="3"/>
       <c r="B45" s="8" t="s">
-        <v>69</v>
+        <v>43</v>
       </c>
       <c r="C45" s="9">
         <v>2</v>
@@ -6713,10 +6776,10 @@
         <v>41602</v>
       </c>
       <c r="E45" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="F45" s="58" t="s">
         <v>69</v>
-      </c>
-      <c r="F45" s="58" t="s">
-        <v>102</v>
       </c>
       <c r="G45" s="38">
         <v>41646</v>
@@ -6765,7 +6828,7 @@
       </c>
       <c r="T45" s="2"/>
     </row>
-    <row r="46" spans="1:20" ht="6.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:20" ht="6.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
@@ -6775,11 +6838,11 @@
       <c r="P46" s="24"/>
       <c r="T46" s="2"/>
     </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B47" s="130" t="s">
-        <v>97</v>
-      </c>
-      <c r="C47" s="131"/>
+    <row r="47" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="B47" s="145" t="s">
+        <v>64</v>
+      </c>
+      <c r="C47" s="146"/>
       <c r="D47" s="1"/>
       <c r="E47" s="1"/>
       <c r="F47" s="1"/>
@@ -6787,11 +6850,11 @@
       <c r="P47" s="24"/>
       <c r="T47" s="2"/>
     </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B48" s="130" t="s">
-        <v>98</v>
-      </c>
-      <c r="C48" s="131"/>
+    <row r="48" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="B48" s="145" t="s">
+        <v>65</v>
+      </c>
+      <c r="C48" s="146"/>
       <c r="D48" s="1"/>
       <c r="E48" s="1"/>
       <c r="F48" s="1"/>
@@ -6799,18 +6862,18 @@
       <c r="P48" s="24"/>
       <c r="T48" s="2"/>
     </row>
-    <row r="49" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B49" s="130" t="s">
-        <v>103</v>
-      </c>
-      <c r="C49" s="131"/>
+    <row r="49" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B49" s="145" t="s">
+        <v>70</v>
+      </c>
+      <c r="C49" s="146"/>
       <c r="D49" s="1"/>
       <c r="E49" s="1"/>
       <c r="F49" s="1"/>
       <c r="G49" s="1"/>
       <c r="T49" s="2"/>
     </row>
-    <row r="50" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
       <c r="D50" s="1"/>
@@ -6819,7 +6882,7 @@
       <c r="G50" s="1"/>
       <c r="T50" s="2"/>
     </row>
-    <row r="51" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
       <c r="D51" s="1"/>
@@ -6828,7 +6891,7 @@
       <c r="G51" s="1"/>
       <c r="T51" s="2"/>
     </row>
-    <row r="52" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
       <c r="D52" s="1"/>
@@ -6837,7 +6900,7 @@
       <c r="G52" s="1"/>
       <c r="T52" s="2"/>
     </row>
-    <row r="53" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
       <c r="D53" s="1"/>
@@ -6848,6 +6911,12 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="G4:S4"/>
     <mergeCell ref="B2:S2"/>
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="F5:F6"/>
@@ -6860,12 +6929,6 @@
     <mergeCell ref="K5:K6"/>
     <mergeCell ref="L5:N5"/>
     <mergeCell ref="O5:S5"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="G5:G6"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="G4:S4"/>
   </mergeCells>
   <pageMargins left="0.45" right="0.45" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="56" fitToHeight="0" orientation="landscape" horizontalDpi="4294967293" r:id="rId1"/>
@@ -6873,30 +6936,30 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:R53"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="T14" sqref="T14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="10.140625" customWidth="1"/>
-    <col min="5" max="5" width="36.140625" customWidth="1"/>
-    <col min="6" max="6" width="10.85546875" customWidth="1"/>
-    <col min="7" max="7" width="9.85546875" customWidth="1"/>
-    <col min="8" max="8" width="9.7109375" customWidth="1"/>
-    <col min="9" max="10" width="10.42578125" customWidth="1"/>
+    <col min="3" max="3" width="10.1640625" customWidth="1"/>
+    <col min="5" max="5" width="36.1640625" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" customWidth="1"/>
+    <col min="7" max="7" width="9.83203125" customWidth="1"/>
+    <col min="8" max="8" width="9.6640625" customWidth="1"/>
+    <col min="9" max="10" width="10.5" customWidth="1"/>
     <col min="11" max="11" width="13" customWidth="1"/>
-    <col min="13" max="13" width="14.5703125" customWidth="1"/>
-    <col min="14" max="14" width="12.140625" customWidth="1"/>
-    <col min="15" max="15" width="10.140625" customWidth="1"/>
-    <col min="17" max="17" width="11.7109375" customWidth="1"/>
-    <col min="18" max="18" width="15.5703125" customWidth="1"/>
+    <col min="13" max="13" width="14.5" customWidth="1"/>
+    <col min="14" max="14" width="12.1640625" customWidth="1"/>
+    <col min="15" max="15" width="10.1640625" customWidth="1"/>
+    <col min="17" max="17" width="11.6640625" customWidth="1"/>
+    <col min="18" max="18" width="15.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" s="2"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -6916,29 +6979,29 @@
       <c r="Q1" s="2"/>
       <c r="R1" s="2"/>
     </row>
-    <row r="2" spans="1:18" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" ht="20" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
-      <c r="B2" s="139" t="s">
-        <v>127</v>
-      </c>
-      <c r="C2" s="140"/>
-      <c r="D2" s="140"/>
-      <c r="E2" s="140"/>
-      <c r="F2" s="140"/>
-      <c r="G2" s="140"/>
-      <c r="H2" s="140"/>
-      <c r="I2" s="140"/>
-      <c r="J2" s="140"/>
-      <c r="K2" s="140"/>
-      <c r="L2" s="140"/>
-      <c r="M2" s="140"/>
-      <c r="N2" s="140"/>
-      <c r="O2" s="140"/>
-      <c r="P2" s="140"/>
-      <c r="Q2" s="140"/>
-      <c r="R2" s="140"/>
-    </row>
-    <row r="3" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="130" t="s">
+        <v>94</v>
+      </c>
+      <c r="C2" s="131"/>
+      <c r="D2" s="131"/>
+      <c r="E2" s="131"/>
+      <c r="F2" s="131"/>
+      <c r="G2" s="131"/>
+      <c r="H2" s="131"/>
+      <c r="I2" s="131"/>
+      <c r="J2" s="131"/>
+      <c r="K2" s="131"/>
+      <c r="L2" s="131"/>
+      <c r="M2" s="131"/>
+      <c r="N2" s="131"/>
+      <c r="O2" s="131"/>
+      <c r="P2" s="131"/>
+      <c r="Q2" s="131"/>
+      <c r="R2" s="131"/>
+    </row>
+    <row r="3" spans="1:18" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -6958,112 +7021,112 @@
       <c r="Q3" s="2"/>
       <c r="R3" s="2"/>
     </row>
-    <row r="4" spans="1:18" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
-      <c r="B4" s="134" t="s">
-        <v>84</v>
-      </c>
-      <c r="C4" s="137"/>
-      <c r="D4" s="137"/>
-      <c r="E4" s="156" t="s">
-        <v>85</v>
-      </c>
-      <c r="F4" s="137"/>
-      <c r="G4" s="137"/>
-      <c r="H4" s="137"/>
-      <c r="I4" s="137"/>
-      <c r="J4" s="137"/>
-      <c r="K4" s="137"/>
-      <c r="L4" s="137"/>
-      <c r="M4" s="137"/>
-      <c r="N4" s="137"/>
-      <c r="O4" s="137"/>
-      <c r="P4" s="137"/>
-      <c r="Q4" s="137"/>
-      <c r="R4" s="138"/>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B4" s="149" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" s="152"/>
+      <c r="D4" s="152"/>
+      <c r="E4" s="154" t="s">
+        <v>53</v>
+      </c>
+      <c r="F4" s="152"/>
+      <c r="G4" s="152"/>
+      <c r="H4" s="152"/>
+      <c r="I4" s="152"/>
+      <c r="J4" s="152"/>
+      <c r="K4" s="152"/>
+      <c r="L4" s="152"/>
+      <c r="M4" s="152"/>
+      <c r="N4" s="152"/>
+      <c r="O4" s="152"/>
+      <c r="P4" s="152"/>
+      <c r="Q4" s="152"/>
+      <c r="R4" s="153"/>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" s="3"/>
-      <c r="B5" s="141" t="s">
+      <c r="B5" s="132" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="145" t="s">
+      <c r="C5" s="136" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="145" t="s">
-        <v>122</v>
-      </c>
-      <c r="E5" s="143" t="s">
-        <v>128</v>
-      </c>
-      <c r="F5" s="132" t="s">
-        <v>125</v>
-      </c>
-      <c r="G5" s="147" t="s">
-        <v>87</v>
-      </c>
-      <c r="H5" s="148" t="s">
-        <v>86</v>
-      </c>
-      <c r="I5" s="148" t="s">
-        <v>81</v>
-      </c>
-      <c r="J5" s="148" t="s">
-        <v>83</v>
-      </c>
-      <c r="K5" s="149" t="s">
-        <v>93</v>
-      </c>
-      <c r="L5" s="150"/>
-      <c r="M5" s="151"/>
-      <c r="N5" s="149" t="s">
-        <v>94</v>
-      </c>
-      <c r="O5" s="152"/>
-      <c r="P5" s="152"/>
-      <c r="Q5" s="152"/>
-      <c r="R5" s="153"/>
-    </row>
-    <row r="6" spans="1:18" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D5" s="136" t="s">
+        <v>89</v>
+      </c>
+      <c r="E5" s="134" t="s">
+        <v>95</v>
+      </c>
+      <c r="F5" s="147" t="s">
+        <v>92</v>
+      </c>
+      <c r="G5" s="138" t="s">
+        <v>55</v>
+      </c>
+      <c r="H5" s="139" t="s">
+        <v>54</v>
+      </c>
+      <c r="I5" s="139" t="s">
+        <v>49</v>
+      </c>
+      <c r="J5" s="139" t="s">
+        <v>51</v>
+      </c>
+      <c r="K5" s="140" t="s">
+        <v>60</v>
+      </c>
+      <c r="L5" s="141"/>
+      <c r="M5" s="142"/>
+      <c r="N5" s="140" t="s">
+        <v>61</v>
+      </c>
+      <c r="O5" s="143"/>
+      <c r="P5" s="143"/>
+      <c r="Q5" s="143"/>
+      <c r="R5" s="144"/>
+    </row>
+    <row r="6" spans="1:18" ht="85" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
-      <c r="B6" s="142"/>
-      <c r="C6" s="146"/>
-      <c r="D6" s="146"/>
-      <c r="E6" s="144"/>
-      <c r="F6" s="133"/>
-      <c r="G6" s="144"/>
-      <c r="H6" s="146"/>
-      <c r="I6" s="146"/>
-      <c r="J6" s="146"/>
+      <c r="B6" s="133"/>
+      <c r="C6" s="137"/>
+      <c r="D6" s="137"/>
+      <c r="E6" s="135"/>
+      <c r="F6" s="148"/>
+      <c r="G6" s="135"/>
+      <c r="H6" s="137"/>
+      <c r="I6" s="137"/>
+      <c r="J6" s="137"/>
       <c r="K6" s="25" t="s">
-        <v>89</v>
+        <v>56</v>
       </c>
       <c r="L6" s="26" t="s">
-        <v>124</v>
+        <v>91</v>
       </c>
       <c r="M6" s="27" t="s">
+        <v>57</v>
+      </c>
+      <c r="N6" s="27" t="s">
+        <v>68</v>
+      </c>
+      <c r="O6" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="P6" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q6" s="27" t="s">
         <v>90</v>
       </c>
-      <c r="N6" s="27" t="s">
-        <v>101</v>
-      </c>
-      <c r="O6" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="P6" s="26" t="s">
-        <v>78</v>
-      </c>
-      <c r="Q6" s="27" t="s">
-        <v>123</v>
-      </c>
       <c r="R6" s="28" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" s="3"/>
       <c r="B7" s="4" t="s">
-        <v>104</v>
+        <v>71</v>
       </c>
       <c r="C7" s="5">
         <v>3</v>
@@ -7118,10 +7181,10 @@
         <v>82.766990291262118</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" s="3"/>
       <c r="B8" s="4" t="s">
-        <v>105</v>
+        <v>72</v>
       </c>
       <c r="C8" s="5">
         <v>3</v>
@@ -7176,10 +7239,10 @@
         <v>99.272727272727295</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" s="3"/>
       <c r="B9" s="12" t="s">
-        <v>106</v>
+        <v>73</v>
       </c>
       <c r="C9" s="13">
         <v>3</v>
@@ -7188,7 +7251,7 @@
         <v>41625</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>99</v>
+        <v>66</v>
       </c>
       <c r="F9" s="36">
         <v>41653</v>
@@ -7236,10 +7299,10 @@
         <v>98.843930635838177</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" s="3"/>
       <c r="B10" s="4" t="s">
-        <v>107</v>
+        <v>74</v>
       </c>
       <c r="C10" s="5">
         <v>3</v>
@@ -7294,10 +7357,10 @@
         <v>99.099099099099277</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" s="3"/>
       <c r="B11" s="4" t="s">
-        <v>108</v>
+        <v>75</v>
       </c>
       <c r="C11" s="5">
         <v>3</v>
@@ -7352,10 +7415,10 @@
         <v>98.837209302325618</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" s="3"/>
       <c r="B12" s="12" t="s">
-        <v>109</v>
+        <v>76</v>
       </c>
       <c r="C12" s="13">
         <v>3</v>
@@ -7410,10 +7473,10 @@
         <v>99.999999999999986</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" s="3"/>
       <c r="B13" s="4" t="s">
-        <v>110</v>
+        <v>77</v>
       </c>
       <c r="C13" s="5">
         <v>3</v>
@@ -7468,10 +7531,10 @@
         <v>100</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14" s="3"/>
       <c r="B14" s="4" t="s">
-        <v>111</v>
+        <v>78</v>
       </c>
       <c r="C14" s="5">
         <v>3</v>
@@ -7526,10 +7589,10 @@
         <v>100</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15" s="3"/>
       <c r="B15" s="12" t="s">
-        <v>112</v>
+        <v>79</v>
       </c>
       <c r="C15" s="13">
         <v>3</v>
@@ -7584,10 +7647,10 @@
         <v>97.916666666666714</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16" s="3"/>
       <c r="B16" s="4" t="s">
-        <v>113</v>
+        <v>80</v>
       </c>
       <c r="C16" s="5">
         <v>3</v>
@@ -7642,10 +7705,10 @@
         <v>100</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A17" s="3"/>
       <c r="B17" s="4" t="s">
-        <v>114</v>
+        <v>81</v>
       </c>
       <c r="C17" s="5">
         <v>3</v>
@@ -7700,10 +7763,10 @@
         <v>99.465240641711148</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A18" s="3"/>
       <c r="B18" s="12" t="s">
-        <v>115</v>
+        <v>82</v>
       </c>
       <c r="C18" s="13">
         <v>3</v>
@@ -7758,10 +7821,10 @@
         <v>99.999999999999986</v>
       </c>
     </row>
-    <row r="19" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="3"/>
       <c r="B19" s="4" t="s">
-        <v>116</v>
+        <v>83</v>
       </c>
       <c r="C19" s="5">
         <v>3</v>
@@ -7770,7 +7833,7 @@
         <v>41625</v>
       </c>
       <c r="E19" s="19" t="s">
-        <v>120</v>
+        <v>87</v>
       </c>
       <c r="F19" s="35">
         <v>41653</v>
@@ -7818,10 +7881,10 @@
         <v>100</v>
       </c>
     </row>
-    <row r="20" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="3"/>
       <c r="B20" s="4" t="s">
-        <v>117</v>
+        <v>84</v>
       </c>
       <c r="C20" s="5">
         <v>3</v>
@@ -7830,7 +7893,7 @@
         <v>41625</v>
       </c>
       <c r="E20" s="19" t="s">
-        <v>126</v>
+        <v>93</v>
       </c>
       <c r="F20" s="35">
         <v>41653</v>
@@ -7878,10 +7941,10 @@
         <v>62.499999999999446</v>
       </c>
     </row>
-    <row r="21" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="3"/>
       <c r="B21" s="12" t="s">
-        <v>118</v>
+        <v>85</v>
       </c>
       <c r="C21" s="13">
         <v>3</v>
@@ -7890,7 +7953,7 @@
         <v>41625</v>
       </c>
       <c r="E21" s="66" t="s">
-        <v>126</v>
+        <v>93</v>
       </c>
       <c r="F21" s="36">
         <v>41653</v>
@@ -7938,7 +8001,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A22" s="3"/>
       <c r="B22" s="4">
         <v>1</v>
@@ -7996,7 +8059,7 @@
         <v>30.553176913855111</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A23" s="3"/>
       <c r="B23" s="4">
         <v>2</v>
@@ -8054,7 +8117,7 @@
         <v>30.962267557320814</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A24" s="3"/>
       <c r="B24" s="12">
         <v>3</v>
@@ -8112,7 +8175,7 @@
         <v>25.394409078328259</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A25" s="3"/>
       <c r="B25" s="4">
         <v>4</v>
@@ -8170,7 +8233,7 @@
         <v>53.378706854642687</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A26" s="3"/>
       <c r="B26" s="4">
         <v>5</v>
@@ -8228,7 +8291,7 @@
         <v>48.781446540880502</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A27" s="3"/>
       <c r="B27" s="12">
         <v>6</v>
@@ -8286,7 +8349,7 @@
         <v>48.929292929292927</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A28" s="3"/>
       <c r="B28" s="4">
         <v>7</v>
@@ -8344,7 +8407,7 @@
         <v>43.127762576299723</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A29" s="3"/>
       <c r="B29" s="4">
         <v>8</v>
@@ -8402,7 +8465,7 @@
         <v>43.038461538461547</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A30" s="3"/>
       <c r="B30" s="12">
         <v>9</v>
@@ -8460,7 +8523,7 @@
         <v>43.857758620689651</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A31" s="3"/>
       <c r="B31" s="4">
         <v>10</v>
@@ -8518,7 +8581,7 @@
         <v>27.324397692568716</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A32" s="3"/>
       <c r="B32" s="4">
         <v>11</v>
@@ -8576,7 +8639,7 @@
         <v>23.284796012068739</v>
       </c>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A33" s="3"/>
       <c r="B33" s="12">
         <v>13</v>
@@ -8634,7 +8697,7 @@
         <v>22.199577294685987</v>
       </c>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A34" s="3"/>
       <c r="B34" s="4">
         <v>14</v>
@@ -8692,7 +8755,7 @@
         <v>20.214597959994702</v>
       </c>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A35" s="3"/>
       <c r="B35" s="4">
         <v>15</v>
@@ -8750,7 +8813,7 @@
         <v>20.291063442734782</v>
       </c>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A36" s="3"/>
       <c r="B36" s="12">
         <v>17</v>
@@ -8808,7 +8871,7 @@
         <v>28.683102826217688</v>
       </c>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A37" s="3"/>
       <c r="B37" s="4">
         <v>18</v>
@@ -8866,7 +8929,7 @@
         <v>31.236194060377979</v>
       </c>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A38" s="3"/>
       <c r="B38" s="4">
         <v>19</v>
@@ -8924,7 +8987,7 @@
         <v>26.060722153050474</v>
       </c>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A39" s="3"/>
       <c r="B39" s="12">
         <v>20</v>
@@ -8982,7 +9045,7 @@
         <v>25.591419406575778</v>
       </c>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A40" s="3"/>
       <c r="B40" s="4">
         <v>21</v>
@@ -9040,7 +9103,7 @@
         <v>29.903774981495186</v>
       </c>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A41" s="3"/>
       <c r="B41" s="4">
         <v>22</v>
@@ -9098,7 +9161,7 @@
         <v>40.846035280013702</v>
       </c>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A42" s="3"/>
       <c r="B42" s="12">
         <v>23</v>
@@ -9156,7 +9219,7 @@
         <v>41.686855091969498</v>
       </c>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A43" s="3"/>
       <c r="B43" s="4">
         <v>24</v>
@@ -9214,7 +9277,7 @@
         <v>39.442970822281161</v>
       </c>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A44" s="3"/>
       <c r="B44" s="4">
         <v>25</v>
@@ -9272,7 +9335,7 @@
         <v>42.180585632238014</v>
       </c>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A45" s="3"/>
       <c r="B45" s="12">
         <v>26</v>
@@ -9330,7 +9393,7 @@
         <v>43.115577889447238</v>
       </c>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A46" s="3"/>
       <c r="B46" s="4">
         <v>27</v>
@@ -9388,7 +9451,7 @@
         <v>44.18628454452405</v>
       </c>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A47" s="3"/>
       <c r="B47" s="4">
         <v>28</v>
@@ -9446,7 +9509,7 @@
         <v>57.472569050321603</v>
       </c>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A48" s="3"/>
       <c r="B48" s="12">
         <v>29</v>
@@ -9504,7 +9567,7 @@
         <v>62.383345297918162</v>
       </c>
     </row>
-    <row r="49" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:18" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A49" s="3"/>
       <c r="B49" s="8">
         <v>30</v>
@@ -9562,12 +9625,12 @@
         <v>63.940698230511714</v>
       </c>
     </row>
-    <row r="50" spans="1:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:18" ht="16" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A50" s="2"/>
-      <c r="B50" s="154" t="s">
-        <v>97</v>
-      </c>
-      <c r="C50" s="155"/>
+      <c r="B50" s="155" t="s">
+        <v>64</v>
+      </c>
+      <c r="C50" s="156"/>
       <c r="D50" s="1"/>
       <c r="E50" s="1"/>
       <c r="F50" s="1"/>
@@ -9584,12 +9647,12 @@
       <c r="Q50" s="2"/>
       <c r="R50" s="2"/>
     </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A51" s="2"/>
-      <c r="B51" s="154" t="s">
-        <v>121</v>
-      </c>
-      <c r="C51" s="155"/>
+      <c r="B51" s="155" t="s">
+        <v>88</v>
+      </c>
+      <c r="C51" s="156"/>
       <c r="D51" s="1"/>
       <c r="E51" s="1"/>
       <c r="F51" s="1"/>
@@ -9606,12 +9669,12 @@
       <c r="Q51" s="2"/>
       <c r="R51" s="2"/>
     </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A52" s="2"/>
-      <c r="B52" s="154" t="s">
-        <v>119</v>
-      </c>
-      <c r="C52" s="155"/>
+      <c r="B52" s="155" t="s">
+        <v>86</v>
+      </c>
+      <c r="C52" s="156"/>
       <c r="D52" s="1"/>
       <c r="E52" s="1"/>
       <c r="F52" s="1"/>
@@ -9628,7 +9691,7 @@
       <c r="Q52" s="2"/>
       <c r="R52" s="2"/>
     </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A53" s="2"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
@@ -9650,6 +9713,13 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="K5:M5"/>
+    <mergeCell ref="N5:R5"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B51:C51"/>
     <mergeCell ref="B2:R2"/>
     <mergeCell ref="B4:D4"/>
     <mergeCell ref="E4:R4"/>
@@ -9660,50 +9730,43 @@
     <mergeCell ref="F5:F6"/>
     <mergeCell ref="G5:G6"/>
     <mergeCell ref="H5:H6"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="J5:J6"/>
-    <mergeCell ref="K5:M5"/>
-    <mergeCell ref="N5:R5"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B51:C51"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:AD62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AC9" sqref="AC9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.5703125" customWidth="1"/>
-    <col min="2" max="2" width="16.85546875" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" customWidth="1"/>
-    <col min="4" max="5" width="11.140625" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" customWidth="1"/>
-    <col min="7" max="7" width="11.140625" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" customWidth="1"/>
-    <col min="9" max="9" width="9.7109375" customWidth="1"/>
-    <col min="10" max="10" width="13.140625" customWidth="1"/>
-    <col min="11" max="11" width="9.7109375" customWidth="1"/>
-    <col min="12" max="16" width="13.140625" customWidth="1"/>
-    <col min="17" max="17" width="12.42578125" customWidth="1"/>
-    <col min="18" max="18" width="15.140625" customWidth="1"/>
-    <col min="19" max="19" width="9.28515625" customWidth="1"/>
-    <col min="20" max="20" width="14.28515625" customWidth="1"/>
-    <col min="21" max="25" width="14.85546875" customWidth="1"/>
+    <col min="1" max="1" width="7.5" customWidth="1"/>
+    <col min="2" max="2" width="16.83203125" customWidth="1"/>
+    <col min="3" max="3" width="10.5" customWidth="1"/>
+    <col min="4" max="5" width="11.1640625" customWidth="1"/>
+    <col min="6" max="6" width="12.83203125" customWidth="1"/>
+    <col min="7" max="7" width="11.1640625" customWidth="1"/>
+    <col min="8" max="8" width="10.6640625" customWidth="1"/>
+    <col min="9" max="9" width="9.6640625" customWidth="1"/>
+    <col min="10" max="10" width="13.1640625" customWidth="1"/>
+    <col min="11" max="11" width="9.6640625" customWidth="1"/>
+    <col min="12" max="16" width="13.1640625" customWidth="1"/>
+    <col min="17" max="17" width="12.5" customWidth="1"/>
+    <col min="18" max="18" width="15.1640625" customWidth="1"/>
+    <col min="19" max="19" width="9.33203125" customWidth="1"/>
+    <col min="20" max="20" width="14.33203125" customWidth="1"/>
+    <col min="21" max="25" width="14.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" ht="6.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -9730,36 +9793,36 @@
       <c r="X1" s="2"/>
       <c r="Y1" s="2"/>
     </row>
-    <row r="2" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
-      <c r="B2" s="139" t="s">
-        <v>132</v>
-      </c>
-      <c r="C2" s="140"/>
-      <c r="D2" s="140"/>
-      <c r="E2" s="140"/>
-      <c r="F2" s="140"/>
-      <c r="G2" s="140"/>
-      <c r="H2" s="140"/>
-      <c r="I2" s="140"/>
-      <c r="J2" s="140"/>
-      <c r="K2" s="140"/>
-      <c r="L2" s="140"/>
-      <c r="M2" s="140"/>
-      <c r="N2" s="140"/>
-      <c r="O2" s="140"/>
-      <c r="P2" s="140"/>
-      <c r="Q2" s="140"/>
-      <c r="R2" s="140"/>
-      <c r="S2" s="140"/>
-      <c r="T2" s="140"/>
-      <c r="U2" s="140"/>
+      <c r="B2" s="130" t="s">
+        <v>99</v>
+      </c>
+      <c r="C2" s="131"/>
+      <c r="D2" s="131"/>
+      <c r="E2" s="131"/>
+      <c r="F2" s="131"/>
+      <c r="G2" s="131"/>
+      <c r="H2" s="131"/>
+      <c r="I2" s="131"/>
+      <c r="J2" s="131"/>
+      <c r="K2" s="131"/>
+      <c r="L2" s="131"/>
+      <c r="M2" s="131"/>
+      <c r="N2" s="131"/>
+      <c r="O2" s="131"/>
+      <c r="P2" s="131"/>
+      <c r="Q2" s="131"/>
+      <c r="R2" s="131"/>
+      <c r="S2" s="131"/>
+      <c r="T2" s="131"/>
+      <c r="U2" s="131"/>
       <c r="V2" s="104"/>
       <c r="W2" s="104"/>
       <c r="X2" s="104"/>
       <c r="Y2" s="104"/>
     </row>
-    <row r="3" spans="1:25" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:25" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -9786,15 +9849,15 @@
       <c r="X3" s="2"/>
       <c r="Y3" s="2"/>
     </row>
-    <row r="4" spans="1:25" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:25" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
-      <c r="B4" s="134" t="s">
-        <v>84</v>
-      </c>
-      <c r="C4" s="137"/>
+      <c r="B4" s="149" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" s="152"/>
       <c r="D4" s="159"/>
       <c r="E4" s="160" t="s">
-        <v>85</v>
+        <v>53</v>
       </c>
       <c r="F4" s="161"/>
       <c r="G4" s="161"/>
@@ -9817,116 +9880,116 @@
       <c r="X4" s="161"/>
       <c r="Y4" s="162"/>
     </row>
-    <row r="5" spans="1:25" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3"/>
       <c r="B5" s="157" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="145" t="s">
+      <c r="C5" s="136" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="145" t="s">
-        <v>122</v>
-      </c>
-      <c r="E5" s="132" t="s">
-        <v>125</v>
-      </c>
-      <c r="F5" s="147" t="s">
-        <v>87</v>
-      </c>
-      <c r="G5" s="148" t="s">
-        <v>86</v>
-      </c>
-      <c r="H5" s="148" t="s">
-        <v>81</v>
-      </c>
-      <c r="I5" s="148" t="s">
-        <v>83</v>
-      </c>
-      <c r="J5" s="149" t="s">
-        <v>93</v>
-      </c>
-      <c r="K5" s="150"/>
-      <c r="L5" s="151"/>
+      <c r="D5" s="136" t="s">
+        <v>89</v>
+      </c>
+      <c r="E5" s="147" t="s">
+        <v>92</v>
+      </c>
+      <c r="F5" s="138" t="s">
+        <v>55</v>
+      </c>
+      <c r="G5" s="139" t="s">
+        <v>54</v>
+      </c>
+      <c r="H5" s="139" t="s">
+        <v>49</v>
+      </c>
+      <c r="I5" s="139" t="s">
+        <v>51</v>
+      </c>
+      <c r="J5" s="140" t="s">
+        <v>60</v>
+      </c>
+      <c r="K5" s="141"/>
+      <c r="L5" s="142"/>
       <c r="M5" s="105"/>
       <c r="N5" s="105"/>
       <c r="O5" s="105"/>
       <c r="P5" s="105"/>
-      <c r="Q5" s="149" t="s">
-        <v>94</v>
-      </c>
-      <c r="R5" s="152"/>
-      <c r="S5" s="152"/>
-      <c r="T5" s="152"/>
-      <c r="U5" s="153"/>
+      <c r="Q5" s="140" t="s">
+        <v>61</v>
+      </c>
+      <c r="R5" s="143"/>
+      <c r="S5" s="143"/>
+      <c r="T5" s="143"/>
+      <c r="U5" s="144"/>
       <c r="V5" s="117"/>
       <c r="W5" s="106"/>
       <c r="X5" s="106"/>
       <c r="Y5" s="118"/>
     </row>
-    <row r="6" spans="1:25" ht="69.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:25" ht="69.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" s="158"/>
-      <c r="C6" s="146"/>
-      <c r="D6" s="146"/>
-      <c r="E6" s="133"/>
-      <c r="F6" s="144"/>
-      <c r="G6" s="146"/>
-      <c r="H6" s="146"/>
-      <c r="I6" s="146"/>
+      <c r="C6" s="137"/>
+      <c r="D6" s="137"/>
+      <c r="E6" s="148"/>
+      <c r="F6" s="135"/>
+      <c r="G6" s="137"/>
+      <c r="H6" s="137"/>
+      <c r="I6" s="137"/>
       <c r="J6" s="25" t="s">
-        <v>89</v>
+        <v>56</v>
       </c>
       <c r="K6" s="26" t="s">
-        <v>124</v>
+        <v>91</v>
       </c>
       <c r="L6" s="27" t="s">
+        <v>57</v>
+      </c>
+      <c r="M6" s="27" t="s">
+        <v>144</v>
+      </c>
+      <c r="N6" s="27" t="s">
+        <v>136</v>
+      </c>
+      <c r="O6" s="27" t="s">
+        <v>137</v>
+      </c>
+      <c r="P6" s="27" t="s">
+        <v>138</v>
+      </c>
+      <c r="Q6" s="27" t="s">
+        <v>68</v>
+      </c>
+      <c r="R6" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="S6" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="T6" s="27" t="s">
         <v>90</v>
       </c>
-      <c r="M6" s="27" t="s">
-        <v>177</v>
-      </c>
-      <c r="N6" s="27" t="s">
-        <v>169</v>
-      </c>
-      <c r="O6" s="27" t="s">
-        <v>170</v>
-      </c>
-      <c r="P6" s="27" t="s">
-        <v>171</v>
-      </c>
-      <c r="Q6" s="27" t="s">
-        <v>101</v>
-      </c>
-      <c r="R6" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="S6" s="26" t="s">
-        <v>78</v>
-      </c>
-      <c r="T6" s="27" t="s">
-        <v>123</v>
-      </c>
       <c r="U6" s="28" t="s">
-        <v>80</v>
+        <v>48</v>
       </c>
       <c r="V6" s="115" t="s">
-        <v>176</v>
+        <v>143</v>
       </c>
       <c r="W6" s="116" t="s">
-        <v>169</v>
+        <v>136</v>
       </c>
       <c r="X6" s="116" t="s">
-        <v>170</v>
+        <v>137</v>
       </c>
       <c r="Y6" s="116" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A7" s="3"/>
       <c r="B7" s="92" t="s">
-        <v>129</v>
+        <v>96</v>
       </c>
       <c r="C7" s="5">
         <v>3</v>
@@ -9994,10 +10057,10 @@
       <c r="X7" s="126"/>
       <c r="Y7" s="119"/>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A8" s="3"/>
       <c r="B8" s="92" t="s">
-        <v>130</v>
+        <v>97</v>
       </c>
       <c r="C8" s="5">
         <v>3</v>
@@ -10083,10 +10146,10 @@
         <v>5.63978218046393E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A9" s="3"/>
       <c r="B9" s="93" t="s">
-        <v>131</v>
+        <v>98</v>
       </c>
       <c r="C9" s="13">
         <v>3</v>
@@ -10154,10 +10217,10 @@
       <c r="X9" s="127"/>
       <c r="Y9" s="119"/>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A10" s="3"/>
       <c r="B10" s="92" t="s">
-        <v>133</v>
+        <v>100</v>
       </c>
       <c r="C10" s="5">
         <v>3</v>
@@ -10225,10 +10288,10 @@
       <c r="X10" s="128"/>
       <c r="Y10" s="120"/>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A11" s="3"/>
       <c r="B11" s="92" t="s">
-        <v>134</v>
+        <v>101</v>
       </c>
       <c r="C11" s="5">
         <v>3</v>
@@ -10314,10 +10377,10 @@
         <v>0.12445699686292314</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A12" s="3"/>
       <c r="B12" s="93" t="s">
-        <v>135</v>
+        <v>102</v>
       </c>
       <c r="C12" s="13">
         <v>3</v>
@@ -10385,10 +10448,10 @@
       <c r="X12" s="127"/>
       <c r="Y12" s="119"/>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A13" s="3"/>
       <c r="B13" s="92" t="s">
-        <v>138</v>
+        <v>105</v>
       </c>
       <c r="C13" s="5">
         <v>3</v>
@@ -10456,10 +10519,10 @@
       <c r="X13" s="128"/>
       <c r="Y13" s="120"/>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A14" s="3"/>
       <c r="B14" s="92" t="s">
-        <v>136</v>
+        <v>103</v>
       </c>
       <c r="C14" s="5">
         <v>3</v>
@@ -10545,10 +10608,10 @@
         <v>5.4287199387934852E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A15" s="3"/>
       <c r="B15" s="93" t="s">
-        <v>137</v>
+        <v>104</v>
       </c>
       <c r="C15" s="13">
         <v>3</v>
@@ -10616,10 +10679,10 @@
       <c r="X15" s="127"/>
       <c r="Y15" s="119"/>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A16" s="3"/>
       <c r="B16" s="92" t="s">
-        <v>139</v>
+        <v>106</v>
       </c>
       <c r="C16" s="5">
         <v>3</v>
@@ -10687,10 +10750,10 @@
       <c r="X16" s="128"/>
       <c r="Y16" s="120"/>
     </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A17" s="3"/>
       <c r="B17" s="92" t="s">
-        <v>141</v>
+        <v>108</v>
       </c>
       <c r="C17" s="5">
         <v>3</v>
@@ -10776,10 +10839,10 @@
         <v>5.1337242396603984E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A18" s="3"/>
       <c r="B18" s="93" t="s">
-        <v>140</v>
+        <v>107</v>
       </c>
       <c r="C18" s="13">
         <v>3</v>
@@ -10847,10 +10910,10 @@
       <c r="X18" s="129"/>
       <c r="Y18" s="121"/>
     </row>
-    <row r="19" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" s="3"/>
       <c r="B19" s="92" t="s">
-        <v>142</v>
+        <v>109</v>
       </c>
       <c r="C19" s="5">
         <v>3</v>
@@ -10912,10 +10975,10 @@
       <c r="X19" s="107"/>
       <c r="Y19" s="107"/>
     </row>
-    <row r="20" spans="1:30" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:30" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="3"/>
       <c r="B20" s="92" t="s">
-        <v>143</v>
+        <v>110</v>
       </c>
       <c r="C20" s="5">
         <v>3</v>
@@ -10977,10 +11040,10 @@
       <c r="X20" s="107"/>
       <c r="Y20" s="107"/>
     </row>
-    <row r="21" spans="1:30" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:30" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="3"/>
       <c r="B21" s="93" t="s">
-        <v>144</v>
+        <v>111</v>
       </c>
       <c r="C21" s="13">
         <v>3</v>
@@ -11042,10 +11105,10 @@
       <c r="X21" s="107"/>
       <c r="Y21" s="107"/>
     </row>
-    <row r="22" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" s="3"/>
       <c r="B22" s="92" t="s">
-        <v>145</v>
+        <v>112</v>
       </c>
       <c r="C22" s="5">
         <v>3</v>
@@ -11110,10 +11173,10 @@
         <v>42003</v>
       </c>
     </row>
-    <row r="23" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" s="3"/>
       <c r="B23" s="93" t="s">
-        <v>146</v>
+        <v>113</v>
       </c>
       <c r="C23" s="13">
         <v>3</v>
@@ -11175,10 +11238,10 @@
       <c r="X23" s="107"/>
       <c r="Y23" s="107"/>
     </row>
-    <row r="24" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" s="3"/>
       <c r="B24" s="92" t="s">
-        <v>147</v>
+        <v>114</v>
       </c>
       <c r="C24" s="5">
         <v>3</v>
@@ -11240,10 +11303,10 @@
       <c r="X24" s="107"/>
       <c r="Y24" s="107"/>
     </row>
-    <row r="25" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" s="3"/>
       <c r="B25" s="93" t="s">
-        <v>148</v>
+        <v>115</v>
       </c>
       <c r="C25" s="13">
         <v>3</v>
@@ -11305,10 +11368,10 @@
       <c r="X25" s="107"/>
       <c r="Y25" s="107"/>
     </row>
-    <row r="26" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" s="3"/>
       <c r="B26" s="94" t="s">
-        <v>149</v>
+        <v>116</v>
       </c>
       <c r="C26" s="84">
         <v>3</v>
@@ -11370,10 +11433,10 @@
       <c r="X26" s="107"/>
       <c r="Y26" s="107"/>
     </row>
-    <row r="27" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" s="3"/>
       <c r="B27" s="93" t="s">
-        <v>150</v>
+        <v>117</v>
       </c>
       <c r="C27" s="13">
         <v>3</v>
@@ -11435,10 +11498,10 @@
       <c r="X27" s="107"/>
       <c r="Y27" s="107"/>
     </row>
-    <row r="28" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" s="3"/>
       <c r="B28" s="92" t="s">
-        <v>151</v>
+        <v>118</v>
       </c>
       <c r="C28" s="5">
         <v>3</v>
@@ -11500,10 +11563,10 @@
       <c r="X28" s="107"/>
       <c r="Y28" s="107"/>
     </row>
-    <row r="29" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" s="3"/>
       <c r="B29" s="92" t="s">
-        <v>152</v>
+        <v>119</v>
       </c>
       <c r="C29" s="5">
         <v>3</v>
@@ -11565,10 +11628,10 @@
       <c r="X29" s="107"/>
       <c r="Y29" s="107"/>
     </row>
-    <row r="30" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" s="3"/>
       <c r="B30" s="93" t="s">
-        <v>153</v>
+        <v>120</v>
       </c>
       <c r="C30" s="13">
         <v>3</v>
@@ -11630,10 +11693,10 @@
       <c r="X30" s="107"/>
       <c r="Y30" s="107"/>
     </row>
-    <row r="31" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" s="3"/>
       <c r="B31" s="92" t="s">
-        <v>154</v>
+        <v>121</v>
       </c>
       <c r="C31" s="5">
         <v>3</v>
@@ -11695,10 +11758,10 @@
       <c r="X31" s="107"/>
       <c r="Y31" s="107"/>
     </row>
-    <row r="32" spans="1:30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" s="3"/>
       <c r="B32" s="92" t="s">
-        <v>155</v>
+        <v>122</v>
       </c>
       <c r="C32" s="5">
         <v>3</v>
@@ -11760,10 +11823,10 @@
       <c r="X32" s="107"/>
       <c r="Y32" s="107"/>
     </row>
-    <row r="33" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" s="3"/>
       <c r="B33" s="93" t="s">
-        <v>156</v>
+        <v>123</v>
       </c>
       <c r="C33" s="13">
         <v>2</v>
@@ -11825,10 +11888,10 @@
       <c r="X33" s="107"/>
       <c r="Y33" s="107"/>
     </row>
-    <row r="34" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" s="3"/>
       <c r="B34" s="92" t="s">
-        <v>157</v>
+        <v>124</v>
       </c>
       <c r="C34" s="5">
         <v>3</v>
@@ -11890,10 +11953,10 @@
       <c r="X34" s="107"/>
       <c r="Y34" s="107"/>
     </row>
-    <row r="35" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" s="3"/>
       <c r="B35" s="92" t="s">
-        <v>159</v>
+        <v>126</v>
       </c>
       <c r="C35" s="5">
         <v>3</v>
@@ -11955,10 +12018,10 @@
       <c r="X35" s="107"/>
       <c r="Y35" s="107"/>
     </row>
-    <row r="36" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" s="3"/>
       <c r="B36" s="93" t="s">
-        <v>158</v>
+        <v>125</v>
       </c>
       <c r="C36" s="13">
         <v>3</v>
@@ -12020,10 +12083,10 @@
       <c r="X36" s="107"/>
       <c r="Y36" s="107"/>
     </row>
-    <row r="37" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" s="3"/>
       <c r="B37" s="92" t="s">
-        <v>160</v>
+        <v>127</v>
       </c>
       <c r="C37" s="5">
         <v>3</v>
@@ -12085,10 +12148,10 @@
       <c r="X37" s="107"/>
       <c r="Y37" s="107"/>
     </row>
-    <row r="38" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" s="3"/>
       <c r="B38" s="92" t="s">
-        <v>161</v>
+        <v>128</v>
       </c>
       <c r="C38" s="5">
         <v>3</v>
@@ -12150,10 +12213,10 @@
       <c r="X38" s="107"/>
       <c r="Y38" s="107"/>
     </row>
-    <row r="39" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" s="3"/>
       <c r="B39" s="93" t="s">
-        <v>162</v>
+        <v>129</v>
       </c>
       <c r="C39" s="13">
         <v>3</v>
@@ -12215,10 +12278,10 @@
       <c r="X39" s="107"/>
       <c r="Y39" s="107"/>
     </row>
-    <row r="40" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" s="3"/>
       <c r="B40" s="92" t="s">
-        <v>163</v>
+        <v>130</v>
       </c>
       <c r="C40" s="5">
         <v>2</v>
@@ -12280,10 +12343,10 @@
       <c r="X40" s="107"/>
       <c r="Y40" s="107"/>
     </row>
-    <row r="41" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41" s="3"/>
       <c r="B41" s="93" t="s">
-        <v>164</v>
+        <v>131</v>
       </c>
       <c r="C41" s="13">
         <v>3</v>
@@ -12345,10 +12408,10 @@
       <c r="X41" s="107"/>
       <c r="Y41" s="107"/>
     </row>
-    <row r="42" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" s="3"/>
       <c r="B42" s="92" t="s">
-        <v>165</v>
+        <v>132</v>
       </c>
       <c r="C42" s="5">
         <v>3</v>
@@ -12410,10 +12473,10 @@
       <c r="X42" s="107"/>
       <c r="Y42" s="107"/>
     </row>
-    <row r="43" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" s="3"/>
       <c r="B43" s="92" t="s">
-        <v>166</v>
+        <v>133</v>
       </c>
       <c r="C43" s="5">
         <v>3</v>
@@ -12475,10 +12538,10 @@
       <c r="X43" s="107"/>
       <c r="Y43" s="107"/>
     </row>
-    <row r="44" spans="1:25" ht="17.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:25" ht="17.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A44" s="3"/>
       <c r="B44" s="95" t="s">
-        <v>167</v>
+        <v>134</v>
       </c>
       <c r="C44" s="9">
         <v>3</v>
@@ -12540,12 +12603,12 @@
       <c r="X44" s="107"/>
       <c r="Y44" s="107"/>
     </row>
-    <row r="45" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A45" s="2"/>
-      <c r="B45" s="154" t="s">
-        <v>97</v>
-      </c>
-      <c r="C45" s="155"/>
+      <c r="B45" s="155" t="s">
+        <v>64</v>
+      </c>
+      <c r="C45" s="156"/>
       <c r="D45" s="1"/>
       <c r="E45" s="1"/>
       <c r="F45" s="2"/>
@@ -12569,12 +12632,12 @@
       <c r="X45" s="2"/>
       <c r="Y45" s="2"/>
     </row>
-    <row r="46" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A46" s="2"/>
-      <c r="B46" s="154" t="s">
-        <v>168</v>
-      </c>
-      <c r="C46" s="155"/>
+      <c r="B46" s="155" t="s">
+        <v>135</v>
+      </c>
+      <c r="C46" s="156"/>
       <c r="D46" s="1"/>
       <c r="E46" s="1"/>
       <c r="F46" s="2"/>
@@ -12598,12 +12661,12 @@
       <c r="X46" s="2"/>
       <c r="Y46" s="2"/>
     </row>
-    <row r="47" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A47" s="2"/>
-      <c r="B47" s="154" t="s">
-        <v>119</v>
-      </c>
-      <c r="C47" s="155"/>
+      <c r="B47" s="155" t="s">
+        <v>86</v>
+      </c>
+      <c r="C47" s="156"/>
       <c r="D47" s="1"/>
       <c r="E47" s="1"/>
       <c r="F47" s="2"/>
@@ -12627,7 +12690,7 @@
       <c r="X47" s="2"/>
       <c r="Y47" s="2"/>
     </row>
-    <row r="48" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A48" s="2"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -12654,51 +12717,51 @@
       <c r="X48" s="2"/>
       <c r="Y48" s="2"/>
     </row>
-    <row r="49" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:24" x14ac:dyDescent="0.2">
       <c r="O49" s="78"/>
       <c r="P49" s="78"/>
       <c r="X49" s="107"/>
     </row>
-    <row r="51" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:24" x14ac:dyDescent="0.2">
       <c r="C51" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="52" spans="2:24" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="52" spans="2:24" x14ac:dyDescent="0.2">
       <c r="C52" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="53" spans="2:24" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="53" spans="2:24" x14ac:dyDescent="0.2">
       <c r="C53" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="54" spans="2:24" x14ac:dyDescent="0.25">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="54" spans="2:24" x14ac:dyDescent="0.2">
       <c r="C54" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="58" spans="2:24" ht="76.5" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="58" spans="2:24" ht="85" x14ac:dyDescent="0.2">
       <c r="B58" s="109" t="s">
-        <v>178</v>
+        <v>145</v>
       </c>
       <c r="C58" s="110" t="s">
-        <v>179</v>
+        <v>146</v>
       </c>
       <c r="D58" s="111" t="s">
-        <v>171</v>
+        <v>138</v>
       </c>
       <c r="E58" s="110" t="s">
-        <v>180</v>
+        <v>147</v>
       </c>
       <c r="F58" s="111" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="59" spans="2:24" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="59" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B59" s="112" t="s">
-        <v>172</v>
+        <v>139</v>
       </c>
       <c r="C59" s="113">
         <v>0.09</v>
@@ -12713,9 +12776,9 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="60" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B60" s="112" t="s">
-        <v>173</v>
+        <v>140</v>
       </c>
       <c r="C60" s="114">
         <v>0.06</v>
@@ -12730,9 +12793,9 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="61" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B61" s="112" t="s">
-        <v>174</v>
+        <v>141</v>
       </c>
       <c r="C61" s="114">
         <v>0.04</v>
@@ -12747,9 +12810,9 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="62" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B62" s="112" t="s">
-        <v>175</v>
+        <v>142</v>
       </c>
       <c r="C62" s="114">
         <v>0.04</v>
@@ -12766,11 +12829,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="G5:G6"/>
-    <mergeCell ref="H5:H6"/>
-    <mergeCell ref="I5:I6"/>
     <mergeCell ref="J5:L5"/>
     <mergeCell ref="Q5:U5"/>
     <mergeCell ref="B45:C45"/>
@@ -12782,6 +12840,11 @@
     <mergeCell ref="F5:F6"/>
     <mergeCell ref="B4:D4"/>
     <mergeCell ref="E4:Y4"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="I5:I6"/>
   </mergeCells>
   <pageMargins left="0.45" right="0.45" top="0.25" bottom="0.25" header="0.3" footer="0.3"/>
   <pageSetup paperSize="17" fitToHeight="0" orientation="landscape" r:id="rId1"/>
@@ -12790,12 +12853,12 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>